<commit_message>
Some comments and refactoring
</commit_message>
<xml_diff>
--- a/Data/result2.xlsx
+++ b/Data/result2.xlsx
@@ -66,7 +66,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -88,6 +88,14 @@
         <v>4540442</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0">
+        <v>4540442</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>